<commit_message>
Processed canopy height profiles
</commit_message>
<xml_diff>
--- a/tally.xlsx
+++ b/tally.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johngodlee/google_drive/phd/thesis/tls/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7831F1-6518-F94D-89FF-592D6EBBB558}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A280ADE-504F-FA48-B27A-526BBDD9A491}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="1" xr2:uid="{E65B02AA-98F5-FA43-B70D-F94208D9632A}"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{E65B02AA-98F5-FA43-B70D-F94208D9632A}"/>
   </bookViews>
   <sheets>
     <sheet name="subplot" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="68">
   <si>
     <t>subplot</t>
   </si>
@@ -239,6 +239,9 @@
   </si>
   <si>
     <t>P15</t>
+  </si>
+  <si>
+    <t>Missing S6,</t>
   </si>
 </sst>
 </file>
@@ -598,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9060313A-6E24-2846-B6EB-79326E1FC092}">
   <dimension ref="A1:L199"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A175" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D189" sqref="D189"/>
     </sheetView>
   </sheetViews>
@@ -7739,8 +7742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E63D1CEB-3449-E94D-A4D9-3E8B33886EFA}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7936,7 +7939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -7947,7 +7950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -7958,7 +7961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -7969,7 +7972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -7980,7 +7983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -7991,7 +7994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -8002,7 +8005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -8011,6 +8014,9 @@
       </c>
       <c r="C23" t="b">
         <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>